<commit_message>
Menambah semua fungsi pada table
</commit_message>
<xml_diff>
--- a/valins_automation/docs/temp.xlsx
+++ b/valins_automation/docs/temp.xlsx
@@ -610,7 +610,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>22990459</t>
+          <t>22990458</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="L4" s="2" t="n">
-        <v>45333.70420138889</v>
+        <v>45334.35872685185</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Menambah flow panel 1 dan panel 2
</commit_message>
<xml_diff>
--- a/valins_automation/docs/temp.xlsx
+++ b/valins_automation/docs/temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\06_python\ppl\valins_automation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB7FCE4-8F46-4D1B-BCC3-4D8857B3F540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72620AF8-03DC-4C8E-A664-ABF4AD95541E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70" yWindow="1850" windowWidth="10640" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="470" yWindow="880" windowWidth="10640" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
   <si>
     <t>No</t>
   </si>
@@ -250,7 +250,19 @@
     <t>ODP-SUD-FAJ/030</t>
   </si>
   <si>
-    <t>ODP-SUD-FBC/051</t>
+    <t>ONT Gagal</t>
+  </si>
+  <si>
+    <t>ODP-SUD-FCL/08</t>
+  </si>
+  <si>
+    <t>ODP-SUD-FBC/074</t>
+  </si>
+  <si>
+    <t>ODP-SUD-FAB/041</t>
+  </si>
+  <si>
+    <t>ODP-SUD-FAZ/041</t>
   </si>
 </sst>
 </file>
@@ -372,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -401,6 +413,9 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1048,10 +1063,10 @@
       <c r="F11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="11" t="s">
+      <c r="G11" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="H11" s="11"/>
       <c r="I11" s="3">
         <v>8</v>
       </c>
@@ -1064,28 +1079,36 @@
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="10">
         <v>7</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="10">
         <v>1</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="G12" s="12">
+        <v>23045811</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="12">
+        <v>16</v>
+      </c>
+      <c r="J12" s="12">
+        <v>3</v>
+      </c>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1104,13 +1127,15 @@
       <c r="F13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1130,9 +1155,15 @@
         <v>24</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="H14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="3">
+        <v>8</v>
+      </c>
+      <c r="J14" s="3">
+        <v>4</v>
+      </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1154,7 +1185,9 @@
       <c r="F15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1180,9 +1213,15 @@
         <v>26</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="H16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="3">
+        <v>8</v>
+      </c>
+      <c r="J16" s="3">
+        <v>4</v>
+      </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1204,7 +1243,9 @@
       <c r="F17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1229,7 +1270,9 @@
       <c r="F18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1254,7 +1297,9 @@
       <c r="F19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -1279,7 +1324,9 @@
       <c r="F20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1305,9 +1352,15 @@
         <v>31</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="H21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="3">
+        <v>8</v>
+      </c>
+      <c r="J21" s="3">
+        <v>2</v>
+      </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>